<commit_message>
+ penambahan tabel simbol dan penamaan excel
</commit_message>
<xml_diff>
--- a/doc/tugas akhir.xlsx
+++ b/doc/tugas akhir.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13245" windowHeight="6945" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13245" windowHeight="6945" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="_Simulasi Batang 2 Penyangga" sheetId="1" r:id="rId1"/>
     <sheet name="SIM 2 Penyangga" sheetId="2" r:id="rId2"/>
     <sheet name="SIM Tali Baja" sheetId="3" r:id="rId3"/>
+    <sheet name="Simbol dan Penamaan" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'_Simulasi Batang 2 Penyangga'!$W$10:$X$10</definedName>
@@ -130,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="184">
   <si>
     <t>Massa (kg)</t>
   </si>
@@ -551,6 +552,138 @@
   <si>
     <t>principal_stress_c0_0(i)</t>
   </si>
+  <si>
+    <t>Kategori</t>
+  </si>
+  <si>
+    <t>Simbol</t>
+  </si>
+  <si>
+    <t>Arti</t>
+  </si>
+  <si>
+    <t>Simulasi Batang Crane</t>
+  </si>
+  <si>
+    <t>Dua Tumpuan</t>
+  </si>
+  <si>
+    <t>Cantilever</t>
+  </si>
+  <si>
+    <t>Tali Baja</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Panjang batang</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Posisi Massa Beban</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Massa Beban</t>
+  </si>
+  <si>
+    <t>Percepatan Gravitasi</t>
+  </si>
+  <si>
+    <t>Ltx</t>
+  </si>
+  <si>
+    <t>Lty</t>
+  </si>
+  <si>
+    <t>Panjang Tali Baja Sumbu x</t>
+  </si>
+  <si>
+    <t>Panjang Tali Baja Sumbu y</t>
+  </si>
+  <si>
+    <t>Pembagi Titik Nodal</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>sigma.y</t>
+  </si>
+  <si>
+    <t>W0</t>
+  </si>
+  <si>
+    <t>Tegangan Yield</t>
+  </si>
+  <si>
+    <t>Massa Per Satuan Panjang</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Tinggi Penampang Batang</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Lebar Penampang Batang</t>
+  </si>
+  <si>
+    <t>t.web</t>
+  </si>
+  <si>
+    <t>t.flange</t>
+  </si>
+  <si>
+    <t>(Lihat Gambar xx)</t>
+  </si>
+  <si>
+    <t>A.section</t>
+  </si>
+  <si>
+    <t>Luas Penampang</t>
+  </si>
+  <si>
+    <t>Referensi</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Gaya Akibat Massa Beban</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Resultan Gaya Akibat Massa Per Satuan Panjang</t>
+  </si>
+  <si>
+    <t>A.x</t>
+  </si>
+  <si>
+    <t>A.y</t>
+  </si>
+  <si>
+    <t>B.y</t>
+  </si>
+  <si>
+    <t>T.x</t>
+  </si>
+  <si>
+    <t>T.y</t>
+  </si>
 </sst>
 </file>
 
@@ -816,7 +949,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -880,6 +1013,28 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -38382,8 +38537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA234"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52918,4 +53073,498 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="48" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="42" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F21" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>